<commit_message>
gitignore update with exact filename that should be ignored in the future
</commit_message>
<xml_diff>
--- a/Esheet.xlsx
+++ b/Esheet.xlsx
@@ -358,10 +358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -376,6 +376,11 @@
         <v>111111</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>22222222</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update gitignore w filename without extension type
</commit_message>
<xml_diff>
--- a/Esheet.xlsx
+++ b/Esheet.xlsx
@@ -358,10 +358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -381,6 +381,11 @@
         <v>22222222</v>
       </c>
     </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>33333</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>